<commit_message>
modified excel quiz format
</commit_message>
<xml_diff>
--- a/sample_exam_files/sample_questions.xlsx
+++ b/sample_exam_files/sample_questions.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07BDC5B3-7200-40D2-9C32-34C72693DF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\razstvien\codes\projects\CSV-ExamInjector\sample_exam_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B135B918-3077-4072-BA4D-F79AB5D8BBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions@trueorfalse" sheetId="1" r:id="rId1"/>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>Questions</t>
   </si>
@@ -103,9 +108,6 @@
     <t>Aengel</t>
   </si>
   <si>
-    <t>What is the specific software that provides feedback on the programming language specific syntax, noticeable errors, warnings and optimization recommendation</t>
-  </si>
-  <si>
     <t>DAP</t>
   </si>
   <si>
@@ -164,6 +166,9 @@
   </si>
   <si>
     <t>Sqlight</t>
+  </si>
+  <si>
+    <t>Index</t>
   </si>
 </sst>
 </file>
@@ -205,11 +210,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EA16EF-B104-4EA3-AE5D-62121FAFDAC9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -639,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="72.75">
+    <row r="2" spans="1:4" ht="75">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -660,340 +677,352 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23C0BC9-1719-4D08-8F30-76385AB08B22}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" ht="30" customHeight="1">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29.25">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:10">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29.25">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:10">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:10">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="43.5">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="30">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="43.5">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="43.5">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="43.5">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC03AA08-D8C5-4ACB-948D-D2F5E54D0C63}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="30" customHeight="1">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29.25">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F4" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="29.25">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29.25">
-      <c r="A5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29.25">
-      <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29.25">
-      <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29.25">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29.25">
-      <c r="A9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="F11" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>